<commit_message>
Cambios en el operador de Reparacion GACEP
</commit_message>
<xml_diff>
--- a/Subresultados/resultadosHistogramaMutacion.xlsx
+++ b/Subresultados/resultadosHistogramaMutacion.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AGEU450" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="GACEPMutacion" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="GACEPReparacionMutacion" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="97">
   <si>
     <t xml:space="preserve">F01</t>
   </si>
@@ -326,6 +327,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -413,11 +415,11 @@
   </sheetPr>
   <dimension ref="A1:CS2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -714,295 +716,295 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
-        <v>193167</v>
+        <v>192630</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>81949</v>
+        <v>81790</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>190142</v>
+        <v>188701</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>222008</v>
+        <v>223666</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>230009</v>
+        <v>228927</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>74161</v>
+        <v>73290.5</v>
       </c>
       <c r="G2" s="1" t="n">
         <v>10153</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>62251</v>
+        <v>62355.5</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>232754</v>
+        <v>232238</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>24710</v>
+        <v>24746.4</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>18339</v>
+        <v>18252.7</v>
       </c>
       <c r="L2" s="1" t="n">
-        <v>56525</v>
+        <v>56447.6</v>
       </c>
       <c r="M2" s="1" t="n">
-        <v>3702</v>
+        <v>3703.5</v>
       </c>
       <c r="N2" s="1" t="n">
-        <v>50131</v>
+        <v>49946.1</v>
       </c>
       <c r="O2" s="1" t="n">
         <v>61494</v>
       </c>
       <c r="P2" s="1" t="n">
-        <v>35692</v>
+        <v>35953.8</v>
       </c>
       <c r="Q2" s="1" t="n">
-        <v>14657</v>
+        <v>14524.9</v>
       </c>
       <c r="R2" s="1" t="n">
-        <v>20185</v>
+        <v>20280.6</v>
       </c>
       <c r="S2" s="1" t="n">
-        <v>35325</v>
+        <v>35033.3</v>
       </c>
       <c r="T2" s="1" t="n">
-        <v>88113</v>
+        <v>88004.1</v>
       </c>
       <c r="U2" s="1" t="n">
-        <v>83712</v>
+        <v>83364.3</v>
       </c>
       <c r="V2" s="1" t="n">
-        <v>104480</v>
+        <v>104608</v>
       </c>
       <c r="W2" s="1" t="n">
-        <v>33459</v>
+        <v>33573.7</v>
       </c>
       <c r="X2" s="1" t="n">
-        <v>105876</v>
+        <v>105713</v>
       </c>
       <c r="Y2" s="1" t="n">
-        <v>56383</v>
+        <v>56002.5</v>
       </c>
       <c r="Z2" s="1" t="n">
-        <v>16080</v>
+        <v>15949.6</v>
       </c>
       <c r="AA2" s="1" t="n">
-        <v>52487</v>
+        <v>52529.1</v>
       </c>
       <c r="AB2" s="1" t="n">
-        <v>53807</v>
+        <v>53674.4</v>
       </c>
       <c r="AC2" s="1" t="n">
-        <v>68480</v>
+        <v>68215.7</v>
       </c>
       <c r="AD2" s="1" t="n">
-        <v>143594</v>
+        <v>143452</v>
       </c>
       <c r="AE2" s="1" t="n">
         <v>188657</v>
       </c>
       <c r="AF2" s="1" t="n">
-        <v>94694</v>
+        <v>94671.5</v>
       </c>
       <c r="AG2" s="1" t="n">
-        <v>60356</v>
+        <v>61645.7</v>
       </c>
       <c r="AH2" s="1" t="n">
-        <v>71912</v>
+        <v>71876</v>
       </c>
       <c r="AI2" s="1" t="n">
-        <v>27543</v>
+        <v>27543.4</v>
       </c>
       <c r="AJ2" s="1" t="n">
-        <v>144921</v>
+        <v>144869</v>
       </c>
       <c r="AK2" s="1" t="n">
-        <v>110704</v>
+        <v>110417</v>
       </c>
       <c r="AL2" s="1" t="n">
-        <v>19417</v>
+        <v>19381.6</v>
       </c>
       <c r="AM2" s="1" t="n">
-        <v>103531</v>
+        <v>104031</v>
       </c>
       <c r="AN2" s="1" t="n">
-        <v>372021</v>
+        <v>376115</v>
       </c>
       <c r="AO2" s="1" t="n">
-        <v>936641</v>
+        <v>936479</v>
       </c>
       <c r="AP2" s="1" t="n">
-        <v>302800</v>
+        <v>302088</v>
       </c>
       <c r="AQ2" s="1" t="n">
-        <v>28973</v>
+        <v>29179.2</v>
       </c>
       <c r="AR2" s="1" t="n">
-        <v>100837</v>
+        <v>100548</v>
       </c>
       <c r="AS2" s="1" t="n">
-        <v>779201</v>
+        <v>779178</v>
       </c>
       <c r="AT2" s="1" t="n">
-        <v>39831</v>
+        <v>40468.6</v>
       </c>
       <c r="AU2" s="1" t="n">
-        <v>692418</v>
+        <v>693113</v>
       </c>
       <c r="AV2" s="1" t="n">
-        <v>778361</v>
+        <v>778717</v>
       </c>
       <c r="AW2" s="1" t="n">
-        <v>622107</v>
+        <v>622530</v>
       </c>
       <c r="AX2" s="1" t="n">
-        <v>48107</v>
+        <v>47941.4</v>
       </c>
       <c r="AY2" s="1" t="n">
-        <v>203418</v>
+        <v>202982</v>
       </c>
       <c r="AZ2" s="1" t="n">
-        <v>238843</v>
+        <v>239154</v>
       </c>
       <c r="BA2" s="1" t="n">
-        <v>219722</v>
+        <v>220645</v>
       </c>
       <c r="BB2" s="1" t="n">
-        <v>186025</v>
+        <v>185475</v>
       </c>
       <c r="BC2" s="1" t="n">
-        <v>80109</v>
+        <v>78900.3</v>
       </c>
       <c r="BD2" s="1" t="n">
-        <v>58754</v>
+        <v>58001.3</v>
       </c>
       <c r="BE2" s="1" t="n">
-        <v>147170</v>
+        <v>147700</v>
       </c>
       <c r="BF2" s="1" t="n">
-        <v>49003</v>
+        <v>48885</v>
       </c>
       <c r="BG2" s="1" t="n">
-        <v>281306</v>
+        <v>281346</v>
       </c>
       <c r="BH2" s="1" t="n">
-        <v>365839</v>
+        <v>368682</v>
       </c>
       <c r="BI2" s="1" t="n">
-        <v>210176</v>
+        <v>209505</v>
       </c>
       <c r="BJ2" s="1" t="n">
-        <v>224751</v>
+        <v>224676</v>
       </c>
       <c r="BK2" s="1" t="n">
-        <v>225369</v>
+        <v>225646</v>
       </c>
       <c r="BL2" s="1" t="n">
-        <v>478963</v>
+        <v>478885</v>
       </c>
       <c r="BM2" s="1" t="n">
-        <v>425883</v>
+        <v>425320</v>
       </c>
       <c r="BN2" s="1" t="n">
-        <v>217763</v>
+        <v>217170</v>
       </c>
       <c r="BO2" s="1" t="n">
-        <v>316534</v>
+        <v>315440</v>
       </c>
       <c r="BP2" s="1" t="n">
-        <v>103438</v>
+        <v>104041</v>
       </c>
       <c r="BQ2" s="1" t="n">
-        <v>139839</v>
+        <v>142199</v>
       </c>
       <c r="BR2" s="1" t="n">
-        <v>440630</v>
+        <v>439128</v>
       </c>
       <c r="BS2" s="1" t="n">
-        <v>282781</v>
+        <v>283127</v>
       </c>
       <c r="BT2" s="1" t="n">
-        <v>60985</v>
+        <v>61507.5</v>
       </c>
       <c r="BU2" s="1" t="n">
-        <v>126145</v>
+        <v>126665</v>
       </c>
       <c r="BV2" s="1" t="n">
-        <v>137690</v>
+        <v>137097</v>
       </c>
       <c r="BW2" s="1" t="n">
-        <v>227583</v>
+        <v>227386</v>
       </c>
       <c r="BX2" s="1" t="n">
-        <v>263331</v>
+        <v>267436</v>
       </c>
       <c r="BY2" s="1" t="n">
-        <v>596190</v>
+        <v>596964</v>
       </c>
       <c r="BZ2" s="1" t="n">
-        <v>514676</v>
+        <v>513040</v>
       </c>
       <c r="CA2" s="1" t="n">
-        <v>377821</v>
+        <v>374916</v>
       </c>
       <c r="CB2" s="1" t="n">
-        <v>28495</v>
+        <v>28698.3</v>
       </c>
       <c r="CC2" s="1" t="n">
-        <v>275059</v>
+        <v>275303</v>
       </c>
       <c r="CD2" s="1" t="n">
-        <v>442681</v>
+        <v>440074</v>
       </c>
       <c r="CE2" s="1" t="n">
-        <v>14777</v>
+        <v>14752.7</v>
       </c>
       <c r="CF2" s="1" t="n">
-        <v>264458</v>
+        <v>263446</v>
       </c>
       <c r="CG2" s="1" t="n">
-        <v>482506</v>
+        <v>481184</v>
       </c>
       <c r="CH2" s="1" t="n">
-        <v>9208</v>
+        <v>9116.6</v>
       </c>
       <c r="CI2" s="1" t="n">
-        <v>245159</v>
+        <v>244729</v>
       </c>
       <c r="CJ2" s="1" t="n">
-        <v>992645</v>
+        <v>990479</v>
       </c>
       <c r="CK2" s="1" t="n">
-        <v>496857</v>
+        <v>500926</v>
       </c>
       <c r="CL2" s="1" t="n">
-        <v>105543</v>
+        <v>104813</v>
       </c>
       <c r="CM2" s="1" t="n">
-        <v>865442</v>
+        <v>866301</v>
       </c>
       <c r="CN2" s="1" t="n">
-        <v>299649</v>
+        <v>303098</v>
       </c>
       <c r="CO2" s="1" t="n">
-        <v>720702</v>
+        <v>715177</v>
       </c>
       <c r="CP2" s="1" t="n">
-        <v>712408</v>
+        <v>723710</v>
       </c>
       <c r="CQ2" s="1" t="n">
-        <v>43295</v>
+        <v>43420.2</v>
       </c>
       <c r="CR2" s="1" t="n">
-        <v>755370</v>
+        <v>754010</v>
       </c>
       <c r="CS2" s="1" t="n">
-        <v>751153</v>
+        <v>752160</v>
       </c>
     </row>
   </sheetData>
@@ -1024,10 +1026,10 @@
   <dimension ref="A1:CS2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.95"/>
   </cols>
@@ -1621,7 +1623,617 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:CS2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD1" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG1" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI1" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN1" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="BO1" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="BS1" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="BT1" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="BU1" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="BV1" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="BW1" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="BX1" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="BY1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="BZ1" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="CA1" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="CB1" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="CC1" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="CD1" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="CE1" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="CF1" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="CG1" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="CH1" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="CI1" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="CJ1" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="CK1" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="CL1" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="CM1" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="CN1" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="CO1" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="CP1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="CQ1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="CR1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="CS1" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>212526</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>79531.7</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>213189</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>244658</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>248467</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>72115.1</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>13197.5</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>65598.8</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>248484</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>26370.2</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>20030.2</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>60477.8</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>4234.2</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>56899.4</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>64455.7</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>38102.4</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>14834.4</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>21250.8</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>37334.4</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <v>99631</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <v>87983.4</v>
+      </c>
+      <c r="V2" s="0" t="n">
+        <v>115638</v>
+      </c>
+      <c r="W2" s="0" t="n">
+        <v>36146.2</v>
+      </c>
+      <c r="X2" s="0" t="n">
+        <v>115302</v>
+      </c>
+      <c r="Y2" s="0" t="n">
+        <v>55284.6</v>
+      </c>
+      <c r="Z2" s="0" t="n">
+        <v>18582.2</v>
+      </c>
+      <c r="AA2" s="0" t="n">
+        <v>54080</v>
+      </c>
+      <c r="AB2" s="0" t="n">
+        <v>52731.7</v>
+      </c>
+      <c r="AC2" s="0" t="n">
+        <v>72656.6</v>
+      </c>
+      <c r="AD2" s="0" t="n">
+        <v>158357</v>
+      </c>
+      <c r="AE2" s="0" t="n">
+        <v>192165</v>
+      </c>
+      <c r="AF2" s="0" t="n">
+        <v>105867</v>
+      </c>
+      <c r="AG2" s="0" t="n">
+        <v>61514.1</v>
+      </c>
+      <c r="AH2" s="0" t="n">
+        <v>76063</v>
+      </c>
+      <c r="AI2" s="0" t="n">
+        <v>29468.8</v>
+      </c>
+      <c r="AJ2" s="0" t="n">
+        <v>161562</v>
+      </c>
+      <c r="AK2" s="0" t="n">
+        <v>121305</v>
+      </c>
+      <c r="AL2" s="0" t="n">
+        <v>21361</v>
+      </c>
+      <c r="AM2" s="0" t="n">
+        <v>119014</v>
+      </c>
+      <c r="AN2" s="0" t="n">
+        <v>313430</v>
+      </c>
+      <c r="AO2" s="0" t="n">
+        <v>983266</v>
+      </c>
+      <c r="AP2" s="0" t="n">
+        <v>253149</v>
+      </c>
+      <c r="AQ2" s="0" t="n">
+        <v>32978.6</v>
+      </c>
+      <c r="AR2" s="0" t="n">
+        <v>94315.9</v>
+      </c>
+      <c r="AS2" s="0" t="n">
+        <v>825296</v>
+      </c>
+      <c r="AT2" s="0" t="n">
+        <v>44124.1</v>
+      </c>
+      <c r="AU2" s="0" t="n">
+        <v>717162</v>
+      </c>
+      <c r="AV2" s="0" t="n">
+        <v>816448</v>
+      </c>
+      <c r="AW2" s="0" t="n">
+        <v>632838</v>
+      </c>
+      <c r="AX2" s="0" t="n">
+        <v>39488.7</v>
+      </c>
+      <c r="AY2" s="0" t="n">
+        <v>206967</v>
+      </c>
+      <c r="AZ2" s="0" t="n">
+        <v>249245</v>
+      </c>
+      <c r="BA2" s="0" t="n">
+        <v>233681</v>
+      </c>
+      <c r="BB2" s="0" t="n">
+        <v>191942</v>
+      </c>
+      <c r="BC2" s="0" t="n">
+        <v>66763.3</v>
+      </c>
+      <c r="BD2" s="0" t="n">
+        <v>50194.9</v>
+      </c>
+      <c r="BE2" s="0" t="n">
+        <v>137753</v>
+      </c>
+      <c r="BF2" s="0" t="n">
+        <v>39433.7</v>
+      </c>
+      <c r="BG2" s="0" t="n">
+        <v>273776</v>
+      </c>
+      <c r="BH2" s="0" t="n">
+        <v>367681</v>
+      </c>
+      <c r="BI2" s="0" t="n">
+        <v>187042</v>
+      </c>
+      <c r="BJ2" s="0" t="n">
+        <v>191384</v>
+      </c>
+      <c r="BK2" s="0" t="n">
+        <v>196566</v>
+      </c>
+      <c r="BL2" s="0" t="n">
+        <v>499320</v>
+      </c>
+      <c r="BM2" s="0" t="n">
+        <v>448356</v>
+      </c>
+      <c r="BN2" s="0" t="n">
+        <v>197810</v>
+      </c>
+      <c r="BO2" s="0" t="n">
+        <v>311635</v>
+      </c>
+      <c r="BP2" s="0" t="n">
+        <v>72945.5</v>
+      </c>
+      <c r="BQ2" s="0" t="n">
+        <v>116643</v>
+      </c>
+      <c r="BR2" s="0" t="n">
+        <v>431662</v>
+      </c>
+      <c r="BS2" s="0" t="n">
+        <v>245982</v>
+      </c>
+      <c r="BT2" s="0" t="n">
+        <v>53478.3</v>
+      </c>
+      <c r="BU2" s="0" t="n">
+        <v>95893</v>
+      </c>
+      <c r="BV2" s="0" t="n">
+        <v>109840</v>
+      </c>
+      <c r="BW2" s="0" t="n">
+        <v>195521</v>
+      </c>
+      <c r="BX2" s="0" t="n">
+        <v>229155</v>
+      </c>
+      <c r="BY2" s="0" t="n">
+        <v>608935</v>
+      </c>
+      <c r="BZ2" s="0" t="n">
+        <v>512333</v>
+      </c>
+      <c r="CA2" s="0" t="n">
+        <v>365222</v>
+      </c>
+      <c r="CB2" s="0" t="n">
+        <v>24338.7</v>
+      </c>
+      <c r="CC2" s="0" t="n">
+        <v>242051</v>
+      </c>
+      <c r="CD2" s="0" t="n">
+        <v>439120</v>
+      </c>
+      <c r="CE2" s="0" t="n">
+        <v>14305.4</v>
+      </c>
+      <c r="CF2" s="0" t="n">
+        <v>225621</v>
+      </c>
+      <c r="CG2" s="0" t="n">
+        <v>491344</v>
+      </c>
+      <c r="CH2" s="0" t="n">
+        <v>9796.2</v>
+      </c>
+      <c r="CI2" s="0" t="n">
+        <v>198785</v>
+      </c>
+      <c r="CJ2" s="0" t="n">
+        <v>1033690</v>
+      </c>
+      <c r="CK2" s="0" t="n">
+        <v>426581</v>
+      </c>
+      <c r="CL2" s="0" t="n">
+        <v>67840.6</v>
+      </c>
+      <c r="CM2" s="0" t="n">
+        <v>885358</v>
+      </c>
+      <c r="CN2" s="0" t="n">
+        <v>221735</v>
+      </c>
+      <c r="CO2" s="0" t="n">
+        <v>694994</v>
+      </c>
+      <c r="CP2" s="0" t="n">
+        <v>698756</v>
+      </c>
+      <c r="CQ2" s="0" t="n">
+        <v>41561.2</v>
+      </c>
+      <c r="CR2" s="0" t="n">
+        <v>729626</v>
+      </c>
+      <c r="CS2" s="0" t="n">
+        <v>725852</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>